<commit_message>
Fix Column Archivo F2002
</commit_message>
<xml_diff>
--- a/WP IVA IIBB.xlsx
+++ b/WP IVA IIBB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D9AAB1-9EE6-4ACF-860D-1778B8995AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AEA82B-932A-41BA-991C-CCD65F4945E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,6 +26,65 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{83AB6C7F-7422-45B8-B145-961B9AC88D3B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Para que el Programa de Procesar Excels lo ejecute se le debe poner SI
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B152C05F-24AF-42D7-9928-54F8882B49A9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Si no se guarda/carga el archivo se debe poner NO</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -110,7 +169,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +183,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -209,6 +281,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,12 +573,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,15 +715,15 @@
         <v>0</v>
       </c>
       <c r="R2" s="6" t="str">
-        <f t="shared" ref="R2:R31" si="9">J2&amp;"Resultados\"&amp;N2&amp;".xlsx"</f>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 2.xlsx</v>
+        <f>J2&amp;"Procesado\"&amp;N2&amp;".xlsx"</f>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 2.xlsx</v>
       </c>
       <c r="S2" s="4">
-        <f t="shared" ref="S2:S31" si="10">IF(D2=D1,1,0)</f>
+        <f t="shared" ref="S2:S31" si="9">IF(D2=D1,1,0)</f>
         <v>0</v>
       </c>
       <c r="T2" s="4">
-        <f t="shared" ref="T2:T31" si="11">IF(D2=D3,1,0)</f>
+        <f t="shared" ref="T2:T31" si="10">IF(D2=D3,1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -657,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B66" si="12">"Cliente "&amp;ROW()</f>
+        <f t="shared" ref="B3:B66" si="11">"Cliente "&amp;ROW()</f>
         <v>Cliente 3</v>
       </c>
       <c r="D3">
@@ -712,15 +788,15 @@
         <v>0</v>
       </c>
       <c r="R3" s="6" t="str">
+        <f t="shared" ref="R3:R66" si="12">J3&amp;"Procesado\"&amp;N3&amp;".xlsx"</f>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 3.xlsx</v>
+      </c>
+      <c r="S3" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 3.xlsx</v>
-      </c>
-      <c r="S3" s="4">
+        <v>1</v>
+      </c>
+      <c r="T3" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T3" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -730,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 4</v>
       </c>
       <c r="D4">
@@ -785,15 +861,15 @@
         <v>0</v>
       </c>
       <c r="R4" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 4.xlsx</v>
+      </c>
+      <c r="S4" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 4.xlsx</v>
-      </c>
-      <c r="S4" s="4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T4" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -803,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 5</v>
       </c>
       <c r="D5">
@@ -858,15 +934,15 @@
         <v>0</v>
       </c>
       <c r="R5" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 5.xlsx</v>
+      </c>
+      <c r="S5" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 5.xlsx</v>
-      </c>
-      <c r="S5" s="4">
+        <v>1</v>
+      </c>
+      <c r="T5" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T5" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -876,7 +952,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 6</v>
       </c>
       <c r="D6">
@@ -931,15 +1007,15 @@
         <v>0</v>
       </c>
       <c r="R6" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 6.xlsx</v>
+      </c>
+      <c r="S6" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 6.xlsx</v>
-      </c>
-      <c r="S6" s="4">
+        <v>1</v>
+      </c>
+      <c r="T6" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T6" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -949,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 7</v>
       </c>
       <c r="D7">
@@ -1004,15 +1080,15 @@
         <v>0</v>
       </c>
       <c r="R7" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 7.xlsx</v>
+      </c>
+      <c r="S7" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 7.xlsx</v>
-      </c>
-      <c r="S7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T7" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1022,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 8</v>
       </c>
       <c r="D8">
@@ -1077,15 +1153,15 @@
         <v>0</v>
       </c>
       <c r="R8" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 8.xlsx</v>
+      </c>
+      <c r="S8" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 8.xlsx</v>
-      </c>
-      <c r="S8" s="4">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T8" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1095,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 9</v>
       </c>
       <c r="D9">
@@ -1150,15 +1226,15 @@
         <v>0</v>
       </c>
       <c r="R9" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 9.xlsx</v>
+      </c>
+      <c r="S9" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 9.xlsx</v>
-      </c>
-      <c r="S9" s="4">
+        <v>1</v>
+      </c>
+      <c r="T9" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T9" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1168,7 +1244,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 10</v>
       </c>
       <c r="D10">
@@ -1223,15 +1299,15 @@
         <v>0</v>
       </c>
       <c r="R10" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 10.xlsx</v>
+      </c>
+      <c r="S10" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 10.xlsx</v>
-      </c>
-      <c r="S10" s="4">
+        <v>1</v>
+      </c>
+      <c r="T10" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T10" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1241,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 11</v>
       </c>
       <c r="D11">
@@ -1296,15 +1372,15 @@
         <v>0</v>
       </c>
       <c r="R11" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 11.xlsx</v>
+      </c>
+      <c r="S11" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 11.xlsx</v>
-      </c>
-      <c r="S11" s="4">
+        <v>1</v>
+      </c>
+      <c r="T11" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T11" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1314,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 12</v>
       </c>
       <c r="D12">
@@ -1369,15 +1445,15 @@
         <v>0</v>
       </c>
       <c r="R12" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 12.xlsx</v>
+      </c>
+      <c r="S12" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 12.xlsx</v>
-      </c>
-      <c r="S12" s="4">
+        <v>1</v>
+      </c>
+      <c r="T12" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T12" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1387,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 13</v>
       </c>
       <c r="D13">
@@ -1442,15 +1518,15 @@
         <v>0</v>
       </c>
       <c r="R13" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 13.xlsx</v>
+      </c>
+      <c r="S13" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 13.xlsx</v>
-      </c>
-      <c r="S13" s="4">
+        <v>1</v>
+      </c>
+      <c r="T13" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T13" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1460,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 14</v>
       </c>
       <c r="D14">
@@ -1515,15 +1591,15 @@
         <v>0</v>
       </c>
       <c r="R14" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 14.xlsx</v>
+      </c>
+      <c r="S14" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 14.xlsx</v>
-      </c>
-      <c r="S14" s="4">
+        <v>1</v>
+      </c>
+      <c r="T14" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T14" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1533,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 15</v>
       </c>
       <c r="D15">
@@ -1588,15 +1664,15 @@
         <v>0</v>
       </c>
       <c r="R15" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 20000000000 - WP IVA - 202307 - Cliente 15.xlsx</v>
+      </c>
+      <c r="S15" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 20000000000 - WP IVA - 202307 - Cliente 15.xlsx</v>
-      </c>
-      <c r="S15" s="4">
+        <v>1</v>
+      </c>
+      <c r="T15" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T15" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1606,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 16</v>
       </c>
       <c r="D16">
@@ -1660,15 +1736,15 @@
         <v>0</v>
       </c>
       <c r="R16" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 16.xlsx</v>
+      </c>
+      <c r="S16" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 16.xlsx</v>
-      </c>
-      <c r="S16" s="4">
+        <v>1</v>
+      </c>
+      <c r="T16" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T16" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1678,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 17</v>
       </c>
       <c r="D17">
@@ -1732,15 +1808,15 @@
         <v>0</v>
       </c>
       <c r="R17" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202303 - Cliente 17.xlsx</v>
+      </c>
+      <c r="S17" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202303 - Cliente 17.xlsx</v>
-      </c>
-      <c r="S17" s="4">
+        <v>1</v>
+      </c>
+      <c r="T17" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T17" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1750,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 18</v>
       </c>
       <c r="D18">
@@ -1804,15 +1880,15 @@
         <v>0</v>
       </c>
       <c r="R18" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 18.xlsx</v>
+      </c>
+      <c r="S18" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 18.xlsx</v>
-      </c>
-      <c r="S18" s="4">
+        <v>1</v>
+      </c>
+      <c r="T18" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T18" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1822,7 +1898,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 19</v>
       </c>
       <c r="D19">
@@ -1876,15 +1952,15 @@
         <v>0</v>
       </c>
       <c r="R19" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 19.xlsx</v>
+      </c>
+      <c r="S19" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 19.xlsx</v>
-      </c>
-      <c r="S19" s="4">
+        <v>1</v>
+      </c>
+      <c r="T19" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T19" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1894,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 20</v>
       </c>
       <c r="D20">
@@ -1948,15 +2024,15 @@
         <v>0</v>
       </c>
       <c r="R20" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202303 - Cliente 20.xlsx</v>
+      </c>
+      <c r="S20" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202303 - Cliente 20.xlsx</v>
-      </c>
-      <c r="S20" s="4">
+        <v>1</v>
+      </c>
+      <c r="T20" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T20" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -1966,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 21</v>
       </c>
       <c r="D21">
@@ -2020,15 +2096,15 @@
         <v>0</v>
       </c>
       <c r="R21" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 21.xlsx</v>
+      </c>
+      <c r="S21" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 21.xlsx</v>
-      </c>
-      <c r="S21" s="4">
+        <v>1</v>
+      </c>
+      <c r="T21" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T21" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2038,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 22</v>
       </c>
       <c r="D22">
@@ -2092,15 +2168,15 @@
         <v>0</v>
       </c>
       <c r="R22" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 22.xlsx</v>
+      </c>
+      <c r="S22" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 22.xlsx</v>
-      </c>
-      <c r="S22" s="4">
+        <v>1</v>
+      </c>
+      <c r="T22" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T22" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2110,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 23</v>
       </c>
       <c r="D23">
@@ -2164,15 +2240,15 @@
         <v>0</v>
       </c>
       <c r="R23" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 23.xlsx</v>
+      </c>
+      <c r="S23" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 23.xlsx</v>
-      </c>
-      <c r="S23" s="4">
+        <v>1</v>
+      </c>
+      <c r="T23" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T23" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2182,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 24</v>
       </c>
       <c r="D24">
@@ -2236,15 +2312,15 @@
         <v>0</v>
       </c>
       <c r="R24" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 24.xlsx</v>
+      </c>
+      <c r="S24" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 24.xlsx</v>
-      </c>
-      <c r="S24" s="4">
+        <v>1</v>
+      </c>
+      <c r="T24" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T24" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2254,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 25</v>
       </c>
       <c r="D25">
@@ -2308,15 +2384,15 @@
         <v>0</v>
       </c>
       <c r="R25" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 25.xlsx</v>
+      </c>
+      <c r="S25" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 25.xlsx</v>
-      </c>
-      <c r="S25" s="4">
+        <v>1</v>
+      </c>
+      <c r="T25" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T25" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2326,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 26</v>
       </c>
       <c r="D26">
@@ -2380,15 +2456,15 @@
         <v>0</v>
       </c>
       <c r="R26" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 26.xlsx</v>
+      </c>
+      <c r="S26" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 26.xlsx</v>
-      </c>
-      <c r="S26" s="4">
+        <v>1</v>
+      </c>
+      <c r="T26" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T26" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2398,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 27</v>
       </c>
       <c r="D27">
@@ -2452,15 +2528,15 @@
         <v>0</v>
       </c>
       <c r="R27" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 27.xlsx</v>
+      </c>
+      <c r="S27" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 27.xlsx</v>
-      </c>
-      <c r="S27" s="4">
+        <v>1</v>
+      </c>
+      <c r="T27" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T27" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2470,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 28</v>
       </c>
       <c r="D28">
@@ -2524,15 +2600,15 @@
         <v>0</v>
       </c>
       <c r="R28" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 28.xlsx</v>
+      </c>
+      <c r="S28" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 28.xlsx</v>
-      </c>
-      <c r="S28" s="4">
+        <v>1</v>
+      </c>
+      <c r="T28" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T28" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2542,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 29</v>
       </c>
       <c r="D29">
@@ -2596,15 +2672,15 @@
         <v>0</v>
       </c>
       <c r="R29" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 29.xlsx</v>
+      </c>
+      <c r="S29" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 29.xlsx</v>
-      </c>
-      <c r="S29" s="4">
+        <v>1</v>
+      </c>
+      <c r="T29" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T29" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2614,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="B30" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 30</v>
       </c>
       <c r="D30">
@@ -2668,15 +2744,15 @@
         <v>0</v>
       </c>
       <c r="R30" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 30.xlsx</v>
+      </c>
+      <c r="S30" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 30.xlsx</v>
-      </c>
-      <c r="S30" s="4">
+        <v>1</v>
+      </c>
+      <c r="T30" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T30" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2686,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="B31" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 31</v>
       </c>
       <c r="D31">
@@ -2740,15 +2816,15 @@
         <v>0</v>
       </c>
       <c r="R31" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 31.xlsx</v>
+      </c>
+      <c r="S31" s="4">
         <f t="shared" si="9"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 31.xlsx</v>
-      </c>
-      <c r="S31" s="4">
+        <v>1</v>
+      </c>
+      <c r="T31" s="4">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="T31" s="4">
-        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -2758,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="B32" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 32</v>
       </c>
       <c r="D32">
@@ -2812,8 +2888,8 @@
         <v>0</v>
       </c>
       <c r="R32" s="6" t="str">
-        <f t="shared" ref="R32" si="22">J32&amp;"Resultados\"&amp;N32&amp;".xlsx"</f>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 32.xlsx</v>
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 32.xlsx</v>
       </c>
       <c r="S32" s="4">
         <f>IF(D32=D31,1,0)</f>
@@ -2830,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 33</v>
       </c>
       <c r="D33">
@@ -2852,57 +2928,57 @@
         <v>14</v>
       </c>
       <c r="J33" s="4" t="str">
-        <f t="shared" ref="J33:J73" si="23">CONCATENATE(I33,YEAR(F33),"\",TEXT(F33,"AAAAMM"),"\Papeles de Trabajo\IVA\")</f>
+        <f t="shared" ref="J33:J73" si="22">CONCATENATE(I33,YEAR(F33),"\",TEXT(F33,"AAAAMM"),"\Papeles de Trabajo\IVA\")</f>
         <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
       </c>
       <c r="K33" s="4" t="str">
-        <f t="shared" ref="K33:K73" si="24">CONCATENATE(I33,YEAR(F33),"\",TEXT(F33,"AAAAMM"),"\Papeles de Trabajo\IIBB\")</f>
+        <f t="shared" ref="K33:K73" si="23">CONCATENATE(I33,YEAR(F33),"\",TEXT(F33,"AAAAMM"),"\Papeles de Trabajo\IIBB\")</f>
         <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
       </c>
       <c r="L33" s="3" t="str">
-        <f t="shared" ref="L33:L73" si="25">UPPER(LEFT(TEXT(F33,"MMMM AAAA"),1))&amp;MID(TEXT(F33,"MMMM AAAA"),2,30)</f>
+        <f t="shared" ref="L33:L73" si="24">UPPER(LEFT(TEXT(F33,"MMMM AAAA"),1))&amp;MID(TEXT(F33,"MMMM AAAA"),2,30)</f>
         <v>Julio 2023</v>
       </c>
       <c r="M33" s="3" t="str">
-        <f t="shared" ref="M33:M73" si="26">YEAR(F33)&amp;TEXT(MONTH(F33),"00")</f>
+        <f t="shared" ref="M33:M73" si="25">YEAR(F33)&amp;TEXT(MONTH(F33),"00")</f>
         <v>202307</v>
       </c>
       <c r="N33" s="3" t="str">
-        <f t="shared" ref="N33:N73" si="27">CONCATENATE(TEXT(A33,"0")," - ",SUBSTITUTE(E33,"-","")," - ","WP IVA - ",TEXT(L33,"AAAAMM")," - ",B33)</f>
+        <f t="shared" ref="N33:N73" si="26">CONCATENATE(TEXT(A33,"0")," - ",SUBSTITUTE(E33,"-","")," - ","WP IVA - ",TEXT(L33,"AAAAMM")," - ",B33)</f>
         <v>0 - 30000000000 - WP IVA - 202307 - Cliente 33</v>
       </c>
       <c r="O33" s="3" t="str">
-        <f t="shared" ref="O33:O73" si="28">CONCATENATE(TEXT(A33,"0")," - ",SUBSTITUTE(E33,"-","")," - ","WP IIBB - ",TEXT(L33,"AAAAMM")," - ",B33)</f>
+        <f t="shared" ref="O33:O73" si="27">CONCATENATE(TEXT(A33,"0")," - ",SUBSTITUTE(E33,"-","")," - ","WP IIBB - ",TEXT(L33,"AAAAMM")," - ",B33)</f>
         <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 33</v>
       </c>
       <c r="P33" s="4">
-        <f t="shared" ref="P33:P73" si="29">ROW(A33)</f>
+        <f t="shared" ref="P33:P73" si="28">ROW(A33)</f>
         <v>33</v>
       </c>
       <c r="Q33" s="4" t="str">
-        <f t="shared" ref="Q33:Q73" si="30">RIGHT(E33,1)</f>
+        <f t="shared" ref="Q33:Q73" si="29">RIGHT(E33,1)</f>
         <v>0</v>
       </c>
       <c r="R33" s="6" t="str">
-        <f t="shared" ref="R33:R73" si="31">J33&amp;"Resultados\"&amp;N33&amp;".xlsx"</f>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 33.xlsx</v>
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 33.xlsx</v>
       </c>
       <c r="S33" s="4">
-        <f t="shared" ref="S33:S73" si="32">IF(D33=D32,1,0)</f>
+        <f t="shared" ref="S33:S73" si="30">IF(D33=D32,1,0)</f>
         <v>1</v>
       </c>
       <c r="T33" s="4">
-        <f t="shared" ref="T33:T73" si="33">IF(D33=D34,1,0)</f>
+        <f t="shared" ref="T33:T73" si="31">IF(D33=D34,1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
-        <f t="shared" ref="A34:A65" si="34">RIGHT(E34,1)</f>
+        <f t="shared" ref="A34:A65" si="32">RIGHT(E34,1)</f>
         <v>0</v>
       </c>
       <c r="B34" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 34</v>
       </c>
       <c r="D34">
@@ -2924,57 +3000,57 @@
         <v>14</v>
       </c>
       <c r="J34" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K34" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K34" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L34" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L34" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M34" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M34" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N34" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N34" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 34</v>
+      </c>
+      <c r="O34" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 34</v>
-      </c>
-      <c r="O34" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 34</v>
+      </c>
+      <c r="P34" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 34</v>
-      </c>
-      <c r="P34" s="4">
+        <v>34</v>
+      </c>
+      <c r="Q34" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>34</v>
-      </c>
-      <c r="Q34" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R34" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 34.xlsx</v>
+      </c>
+      <c r="S34" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R34" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T34" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 34.xlsx</v>
-      </c>
-      <c r="S34" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T34" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 35</v>
       </c>
       <c r="D35">
@@ -2996,57 +3072,57 @@
         <v>14</v>
       </c>
       <c r="J35" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K35" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K35" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L35" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L35" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M35" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M35" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N35" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N35" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 35</v>
+      </c>
+      <c r="O35" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 35</v>
-      </c>
-      <c r="O35" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 35</v>
+      </c>
+      <c r="P35" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 35</v>
-      </c>
-      <c r="P35" s="4">
+        <v>35</v>
+      </c>
+      <c r="Q35" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>35</v>
-      </c>
-      <c r="Q35" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R35" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 35.xlsx</v>
+      </c>
+      <c r="S35" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R35" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T35" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 35.xlsx</v>
-      </c>
-      <c r="S35" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T35" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 36</v>
       </c>
       <c r="D36">
@@ -3068,57 +3144,57 @@
         <v>14</v>
       </c>
       <c r="J36" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K36" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K36" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L36" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L36" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M36" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M36" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N36" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N36" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 36</v>
+      </c>
+      <c r="O36" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 36</v>
-      </c>
-      <c r="O36" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 36</v>
+      </c>
+      <c r="P36" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 36</v>
-      </c>
-      <c r="P36" s="4">
+        <v>36</v>
+      </c>
+      <c r="Q36" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>36</v>
-      </c>
-      <c r="Q36" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R36" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 36.xlsx</v>
+      </c>
+      <c r="S36" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R36" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T36" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 36.xlsx</v>
-      </c>
-      <c r="S36" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T36" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B37" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 37</v>
       </c>
       <c r="D37">
@@ -3140,57 +3216,57 @@
         <v>14</v>
       </c>
       <c r="J37" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K37" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K37" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L37" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L37" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M37" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M37" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N37" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N37" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 37</v>
+      </c>
+      <c r="O37" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 37</v>
-      </c>
-      <c r="O37" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 37</v>
+      </c>
+      <c r="P37" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 37</v>
-      </c>
-      <c r="P37" s="4">
+        <v>37</v>
+      </c>
+      <c r="Q37" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>37</v>
-      </c>
-      <c r="Q37" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R37" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 37.xlsx</v>
+      </c>
+      <c r="S37" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R37" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T37" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 37.xlsx</v>
-      </c>
-      <c r="S37" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T37" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 38</v>
       </c>
       <c r="D38">
@@ -3212,57 +3288,57 @@
         <v>14</v>
       </c>
       <c r="J38" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K38" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K38" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L38" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L38" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M38" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M38" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N38" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N38" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 38</v>
+      </c>
+      <c r="O38" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 38</v>
-      </c>
-      <c r="O38" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 38</v>
+      </c>
+      <c r="P38" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 38</v>
-      </c>
-      <c r="P38" s="4">
+        <v>38</v>
+      </c>
+      <c r="Q38" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>38</v>
-      </c>
-      <c r="Q38" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R38" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 38.xlsx</v>
+      </c>
+      <c r="S38" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R38" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T38" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 38.xlsx</v>
-      </c>
-      <c r="S38" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T38" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B39" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 39</v>
       </c>
       <c r="D39">
@@ -3284,57 +3360,57 @@
         <v>14</v>
       </c>
       <c r="J39" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K39" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K39" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L39" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L39" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M39" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M39" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N39" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N39" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 39</v>
+      </c>
+      <c r="O39" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 39</v>
-      </c>
-      <c r="O39" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 39</v>
+      </c>
+      <c r="P39" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 39</v>
-      </c>
-      <c r="P39" s="4">
+        <v>39</v>
+      </c>
+      <c r="Q39" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>39</v>
-      </c>
-      <c r="Q39" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R39" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 39.xlsx</v>
+      </c>
+      <c r="S39" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R39" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T39" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 39.xlsx</v>
-      </c>
-      <c r="S39" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T39" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 40</v>
       </c>
       <c r="D40">
@@ -3356,57 +3432,57 @@
         <v>14</v>
       </c>
       <c r="J40" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K40" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K40" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L40" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L40" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M40" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M40" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N40" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N40" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 40</v>
+      </c>
+      <c r="O40" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 40</v>
-      </c>
-      <c r="O40" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 40</v>
+      </c>
+      <c r="P40" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 40</v>
-      </c>
-      <c r="P40" s="4">
+        <v>40</v>
+      </c>
+      <c r="Q40" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>40</v>
-      </c>
-      <c r="Q40" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R40" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 40.xlsx</v>
+      </c>
+      <c r="S40" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R40" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T40" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 40.xlsx</v>
-      </c>
-      <c r="S40" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T40" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 41</v>
       </c>
       <c r="D41">
@@ -3428,57 +3504,57 @@
         <v>14</v>
       </c>
       <c r="J41" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K41" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K41" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L41" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L41" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M41" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M41" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N41" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N41" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 41</v>
+      </c>
+      <c r="O41" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 41</v>
-      </c>
-      <c r="O41" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 41</v>
+      </c>
+      <c r="P41" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 41</v>
-      </c>
-      <c r="P41" s="4">
+        <v>41</v>
+      </c>
+      <c r="Q41" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>41</v>
-      </c>
-      <c r="Q41" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R41" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 41.xlsx</v>
+      </c>
+      <c r="S41" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R41" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T41" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 41.xlsx</v>
-      </c>
-      <c r="S41" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T41" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 42</v>
       </c>
       <c r="D42">
@@ -3500,57 +3576,57 @@
         <v>14</v>
       </c>
       <c r="J42" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K42" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K42" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L42" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L42" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M42" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M42" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N42" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N42" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 42</v>
+      </c>
+      <c r="O42" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 42</v>
-      </c>
-      <c r="O42" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 42</v>
+      </c>
+      <c r="P42" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 42</v>
-      </c>
-      <c r="P42" s="4">
+        <v>42</v>
+      </c>
+      <c r="Q42" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>42</v>
-      </c>
-      <c r="Q42" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R42" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 42.xlsx</v>
+      </c>
+      <c r="S42" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R42" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T42" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 42.xlsx</v>
-      </c>
-      <c r="S42" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T42" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 43</v>
       </c>
       <c r="D43">
@@ -3572,57 +3648,57 @@
         <v>14</v>
       </c>
       <c r="J43" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K43" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K43" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L43" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L43" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M43" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M43" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N43" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N43" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 43</v>
+      </c>
+      <c r="O43" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 43</v>
-      </c>
-      <c r="O43" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 43</v>
+      </c>
+      <c r="P43" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 43</v>
-      </c>
-      <c r="P43" s="4">
+        <v>43</v>
+      </c>
+      <c r="Q43" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>43</v>
-      </c>
-      <c r="Q43" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R43" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 43.xlsx</v>
+      </c>
+      <c r="S43" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R43" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T43" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 43.xlsx</v>
-      </c>
-      <c r="S43" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T43" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 44</v>
       </c>
       <c r="D44">
@@ -3644,57 +3720,57 @@
         <v>14</v>
       </c>
       <c r="J44" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K44" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K44" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L44" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L44" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M44" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M44" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N44" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N44" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 44</v>
+      </c>
+      <c r="O44" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 44</v>
-      </c>
-      <c r="O44" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 44</v>
+      </c>
+      <c r="P44" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 44</v>
-      </c>
-      <c r="P44" s="4">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>44</v>
-      </c>
-      <c r="Q44" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R44" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 44.xlsx</v>
+      </c>
+      <c r="S44" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R44" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T44" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 44.xlsx</v>
-      </c>
-      <c r="S44" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T44" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 45</v>
       </c>
       <c r="D45">
@@ -3716,57 +3792,57 @@
         <v>14</v>
       </c>
       <c r="J45" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K45" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K45" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L45" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L45" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M45" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M45" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N45" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N45" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 45</v>
+      </c>
+      <c r="O45" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 45</v>
-      </c>
-      <c r="O45" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 45</v>
+      </c>
+      <c r="P45" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 45</v>
-      </c>
-      <c r="P45" s="4">
+        <v>45</v>
+      </c>
+      <c r="Q45" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>45</v>
-      </c>
-      <c r="Q45" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R45" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 45.xlsx</v>
+      </c>
+      <c r="S45" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R45" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T45" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 45.xlsx</v>
-      </c>
-      <c r="S45" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T45" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B46" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 46</v>
       </c>
       <c r="D46">
@@ -3788,57 +3864,57 @@
         <v>14</v>
       </c>
       <c r="J46" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K46" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K46" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L46" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L46" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M46" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M46" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N46" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N46" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 46</v>
+      </c>
+      <c r="O46" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 46</v>
-      </c>
-      <c r="O46" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 46</v>
+      </c>
+      <c r="P46" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 46</v>
-      </c>
-      <c r="P46" s="4">
+        <v>46</v>
+      </c>
+      <c r="Q46" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>46</v>
-      </c>
-      <c r="Q46" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R46" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 46.xlsx</v>
+      </c>
+      <c r="S46" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R46" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T46" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 46.xlsx</v>
-      </c>
-      <c r="S46" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T46" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B47" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 47</v>
       </c>
       <c r="D47">
@@ -3860,57 +3936,57 @@
         <v>14</v>
       </c>
       <c r="J47" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K47" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K47" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L47" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L47" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M47" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M47" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N47" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N47" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 47</v>
+      </c>
+      <c r="O47" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 47</v>
-      </c>
-      <c r="O47" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 47</v>
+      </c>
+      <c r="P47" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 47</v>
-      </c>
-      <c r="P47" s="4">
+        <v>47</v>
+      </c>
+      <c r="Q47" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>47</v>
-      </c>
-      <c r="Q47" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R47" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 47.xlsx</v>
+      </c>
+      <c r="S47" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R47" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T47" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 47.xlsx</v>
-      </c>
-      <c r="S47" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T47" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 48</v>
       </c>
       <c r="D48">
@@ -3932,57 +4008,57 @@
         <v>14</v>
       </c>
       <c r="J48" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K48" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K48" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L48" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L48" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M48" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M48" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N48" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N48" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 48</v>
+      </c>
+      <c r="O48" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 48</v>
-      </c>
-      <c r="O48" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 48</v>
+      </c>
+      <c r="P48" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 48</v>
-      </c>
-      <c r="P48" s="4">
+        <v>48</v>
+      </c>
+      <c r="Q48" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>48</v>
-      </c>
-      <c r="Q48" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R48" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 48.xlsx</v>
+      </c>
+      <c r="S48" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R48" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T48" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 48.xlsx</v>
-      </c>
-      <c r="S48" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T48" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 49</v>
       </c>
       <c r="D49">
@@ -4004,57 +4080,57 @@
         <v>14</v>
       </c>
       <c r="J49" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K49" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K49" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L49" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L49" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M49" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M49" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N49" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N49" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 49</v>
+      </c>
+      <c r="O49" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 49</v>
-      </c>
-      <c r="O49" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 49</v>
+      </c>
+      <c r="P49" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 49</v>
-      </c>
-      <c r="P49" s="4">
+        <v>49</v>
+      </c>
+      <c r="Q49" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>49</v>
-      </c>
-      <c r="Q49" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R49" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 49.xlsx</v>
+      </c>
+      <c r="S49" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R49" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T49" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 49.xlsx</v>
-      </c>
-      <c r="S49" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T49" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 50</v>
       </c>
       <c r="D50">
@@ -4076,57 +4152,57 @@
         <v>14</v>
       </c>
       <c r="J50" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K50" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K50" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L50" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L50" s="3" t="str">
+        <v>Marzo 2023</v>
+      </c>
+      <c r="M50" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Marzo 2023</v>
-      </c>
-      <c r="M50" s="3" t="str">
+        <v>202303</v>
+      </c>
+      <c r="N50" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202303</v>
-      </c>
-      <c r="N50" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202303 - Cliente 50</v>
+      </c>
+      <c r="O50" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202303 - Cliente 50</v>
-      </c>
-      <c r="O50" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202303 - Cliente 50</v>
+      </c>
+      <c r="P50" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202303 - Cliente 50</v>
-      </c>
-      <c r="P50" s="4">
+        <v>50</v>
+      </c>
+      <c r="Q50" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>50</v>
-      </c>
-      <c r="Q50" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R50" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202303 - Cliente 50.xlsx</v>
+      </c>
+      <c r="S50" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R50" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T50" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202303\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202303 - Cliente 50.xlsx</v>
-      </c>
-      <c r="S50" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T50" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 51</v>
       </c>
       <c r="D51">
@@ -4148,57 +4224,57 @@
         <v>14</v>
       </c>
       <c r="J51" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K51" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K51" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L51" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L51" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M51" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M51" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N51" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N51" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 51</v>
+      </c>
+      <c r="O51" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 51</v>
-      </c>
-      <c r="O51" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 51</v>
+      </c>
+      <c r="P51" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 51</v>
-      </c>
-      <c r="P51" s="4">
+        <v>51</v>
+      </c>
+      <c r="Q51" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>51</v>
-      </c>
-      <c r="Q51" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R51" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 51.xlsx</v>
+      </c>
+      <c r="S51" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R51" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T51" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 51.xlsx</v>
-      </c>
-      <c r="S51" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T51" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B52" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 52</v>
       </c>
       <c r="D52">
@@ -4220,57 +4296,57 @@
         <v>14</v>
       </c>
       <c r="J52" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K52" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K52" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L52" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L52" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M52" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M52" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N52" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N52" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 52</v>
+      </c>
+      <c r="O52" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 52</v>
-      </c>
-      <c r="O52" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 52</v>
+      </c>
+      <c r="P52" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 52</v>
-      </c>
-      <c r="P52" s="4">
+        <v>52</v>
+      </c>
+      <c r="Q52" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>52</v>
-      </c>
-      <c r="Q52" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R52" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 52.xlsx</v>
+      </c>
+      <c r="S52" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R52" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T52" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 52.xlsx</v>
-      </c>
-      <c r="S52" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T52" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B53" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 53</v>
       </c>
       <c r="D53">
@@ -4292,57 +4368,57 @@
         <v>14</v>
       </c>
       <c r="J53" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K53" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K53" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L53" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L53" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M53" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M53" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N53" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N53" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 53</v>
+      </c>
+      <c r="O53" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 53</v>
-      </c>
-      <c r="O53" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 53</v>
+      </c>
+      <c r="P53" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 53</v>
-      </c>
-      <c r="P53" s="4">
+        <v>53</v>
+      </c>
+      <c r="Q53" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>53</v>
-      </c>
-      <c r="Q53" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R53" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 53.xlsx</v>
+      </c>
+      <c r="S53" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R53" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T53" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 53.xlsx</v>
-      </c>
-      <c r="S53" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T53" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B54" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 54</v>
       </c>
       <c r="D54">
@@ -4364,57 +4440,57 @@
         <v>14</v>
       </c>
       <c r="J54" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K54" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K54" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L54" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L54" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M54" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M54" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N54" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N54" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 54</v>
+      </c>
+      <c r="O54" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 54</v>
-      </c>
-      <c r="O54" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 54</v>
+      </c>
+      <c r="P54" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 54</v>
-      </c>
-      <c r="P54" s="4">
+        <v>54</v>
+      </c>
+      <c r="Q54" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>54</v>
-      </c>
-      <c r="Q54" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R54" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 54.xlsx</v>
+      </c>
+      <c r="S54" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R54" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T54" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 54.xlsx</v>
-      </c>
-      <c r="S54" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T54" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B55" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 55</v>
       </c>
       <c r="D55">
@@ -4436,57 +4512,57 @@
         <v>14</v>
       </c>
       <c r="J55" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K55" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K55" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L55" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L55" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M55" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M55" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N55" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N55" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 55</v>
+      </c>
+      <c r="O55" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 55</v>
-      </c>
-      <c r="O55" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 55</v>
+      </c>
+      <c r="P55" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 55</v>
-      </c>
-      <c r="P55" s="4">
+        <v>55</v>
+      </c>
+      <c r="Q55" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>55</v>
-      </c>
-      <c r="Q55" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R55" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 55.xlsx</v>
+      </c>
+      <c r="S55" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R55" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T55" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 55.xlsx</v>
-      </c>
-      <c r="S55" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T55" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B56" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 56</v>
       </c>
       <c r="D56">
@@ -4508,57 +4584,57 @@
         <v>14</v>
       </c>
       <c r="J56" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K56" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K56" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L56" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L56" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M56" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M56" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N56" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N56" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 56</v>
+      </c>
+      <c r="O56" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 56</v>
-      </c>
-      <c r="O56" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 56</v>
+      </c>
+      <c r="P56" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 56</v>
-      </c>
-      <c r="P56" s="4">
+        <v>56</v>
+      </c>
+      <c r="Q56" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>56</v>
-      </c>
-      <c r="Q56" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R56" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 56.xlsx</v>
+      </c>
+      <c r="S56" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R56" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T56" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 56.xlsx</v>
-      </c>
-      <c r="S56" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T56" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B57" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 57</v>
       </c>
       <c r="D57">
@@ -4580,57 +4656,57 @@
         <v>14</v>
       </c>
       <c r="J57" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K57" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K57" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L57" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L57" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M57" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M57" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N57" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N57" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 57</v>
+      </c>
+      <c r="O57" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 57</v>
-      </c>
-      <c r="O57" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 57</v>
+      </c>
+      <c r="P57" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 57</v>
-      </c>
-      <c r="P57" s="4">
+        <v>57</v>
+      </c>
+      <c r="Q57" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>57</v>
-      </c>
-      <c r="Q57" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R57" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 57.xlsx</v>
+      </c>
+      <c r="S57" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R57" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T57" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 57.xlsx</v>
-      </c>
-      <c r="S57" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T57" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B58" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 58</v>
       </c>
       <c r="D58">
@@ -4652,57 +4728,57 @@
         <v>14</v>
       </c>
       <c r="J58" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K58" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K58" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L58" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L58" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M58" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M58" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N58" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N58" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 58</v>
+      </c>
+      <c r="O58" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 58</v>
-      </c>
-      <c r="O58" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 58</v>
+      </c>
+      <c r="P58" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 58</v>
-      </c>
-      <c r="P58" s="4">
+        <v>58</v>
+      </c>
+      <c r="Q58" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>58</v>
-      </c>
-      <c r="Q58" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R58" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 58.xlsx</v>
+      </c>
+      <c r="S58" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R58" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T58" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 58.xlsx</v>
-      </c>
-      <c r="S58" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T58" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B59" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 59</v>
       </c>
       <c r="D59">
@@ -4724,57 +4800,57 @@
         <v>14</v>
       </c>
       <c r="J59" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K59" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K59" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L59" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L59" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M59" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M59" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N59" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N59" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 59</v>
+      </c>
+      <c r="O59" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 59</v>
-      </c>
-      <c r="O59" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 59</v>
+      </c>
+      <c r="P59" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 59</v>
-      </c>
-      <c r="P59" s="4">
+        <v>59</v>
+      </c>
+      <c r="Q59" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>59</v>
-      </c>
-      <c r="Q59" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R59" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 59.xlsx</v>
+      </c>
+      <c r="S59" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R59" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T59" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 59.xlsx</v>
-      </c>
-      <c r="S59" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T59" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B60" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 60</v>
       </c>
       <c r="D60">
@@ -4796,57 +4872,57 @@
         <v>14</v>
       </c>
       <c r="J60" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K60" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K60" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L60" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L60" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M60" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M60" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N60" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N60" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 60</v>
+      </c>
+      <c r="O60" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 60</v>
-      </c>
-      <c r="O60" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 60</v>
+      </c>
+      <c r="P60" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 60</v>
-      </c>
-      <c r="P60" s="4">
+        <v>60</v>
+      </c>
+      <c r="Q60" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>60</v>
-      </c>
-      <c r="Q60" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R60" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 60.xlsx</v>
+      </c>
+      <c r="S60" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R60" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T60" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 60.xlsx</v>
-      </c>
-      <c r="S60" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T60" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B61" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 61</v>
       </c>
       <c r="D61">
@@ -4868,57 +4944,57 @@
         <v>14</v>
       </c>
       <c r="J61" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K61" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K61" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L61" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L61" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M61" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M61" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N61" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N61" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 61</v>
+      </c>
+      <c r="O61" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 61</v>
-      </c>
-      <c r="O61" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 61</v>
+      </c>
+      <c r="P61" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 61</v>
-      </c>
-      <c r="P61" s="4">
+        <v>61</v>
+      </c>
+      <c r="Q61" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>61</v>
-      </c>
-      <c r="Q61" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R61" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 61.xlsx</v>
+      </c>
+      <c r="S61" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R61" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T61" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 61.xlsx</v>
-      </c>
-      <c r="S61" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T61" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B62" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 62</v>
       </c>
       <c r="D62">
@@ -4940,57 +5016,57 @@
         <v>14</v>
       </c>
       <c r="J62" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K62" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K62" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L62" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L62" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M62" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M62" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N62" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N62" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 62</v>
+      </c>
+      <c r="O62" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 62</v>
-      </c>
-      <c r="O62" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 62</v>
+      </c>
+      <c r="P62" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 62</v>
-      </c>
-      <c r="P62" s="4">
+        <v>62</v>
+      </c>
+      <c r="Q62" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>62</v>
-      </c>
-      <c r="Q62" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R62" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 62.xlsx</v>
+      </c>
+      <c r="S62" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R62" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T62" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 62.xlsx</v>
-      </c>
-      <c r="S62" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T62" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B63" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 63</v>
       </c>
       <c r="D63">
@@ -5012,57 +5088,57 @@
         <v>14</v>
       </c>
       <c r="J63" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K63" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K63" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L63" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L63" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M63" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M63" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N63" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N63" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 63</v>
+      </c>
+      <c r="O63" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 63</v>
-      </c>
-      <c r="O63" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 63</v>
+      </c>
+      <c r="P63" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 63</v>
-      </c>
-      <c r="P63" s="4">
+        <v>63</v>
+      </c>
+      <c r="Q63" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>63</v>
-      </c>
-      <c r="Q63" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R63" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 63.xlsx</v>
+      </c>
+      <c r="S63" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R63" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T63" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 63.xlsx</v>
-      </c>
-      <c r="S63" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T63" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B64" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 64</v>
       </c>
       <c r="D64">
@@ -5084,57 +5160,57 @@
         <v>14</v>
       </c>
       <c r="J64" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K64" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K64" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L64" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L64" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M64" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M64" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N64" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N64" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 64</v>
+      </c>
+      <c r="O64" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 64</v>
-      </c>
-      <c r="O64" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 64</v>
+      </c>
+      <c r="P64" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 64</v>
-      </c>
-      <c r="P64" s="4">
+        <v>64</v>
+      </c>
+      <c r="Q64" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>64</v>
-      </c>
-      <c r="Q64" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R64" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 64.xlsx</v>
+      </c>
+      <c r="S64" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R64" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T64" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 64.xlsx</v>
-      </c>
-      <c r="S64" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T64" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="B65" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 65</v>
       </c>
       <c r="D65">
@@ -5156,57 +5232,57 @@
         <v>14</v>
       </c>
       <c r="J65" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K65" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K65" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L65" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L65" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M65" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M65" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N65" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N65" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 65</v>
+      </c>
+      <c r="O65" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 65</v>
-      </c>
-      <c r="O65" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 65</v>
+      </c>
+      <c r="P65" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 65</v>
-      </c>
-      <c r="P65" s="4">
+        <v>65</v>
+      </c>
+      <c r="Q65" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>65</v>
-      </c>
-      <c r="Q65" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R65" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 65.xlsx</v>
+      </c>
+      <c r="S65" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R65" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T65" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 65.xlsx</v>
-      </c>
-      <c r="S65" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T65" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
-        <f t="shared" ref="A66:A73" si="35">RIGHT(E66,1)</f>
+        <f t="shared" ref="A66:A73" si="33">RIGHT(E66,1)</f>
         <v>0</v>
       </c>
       <c r="B66" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Cliente 66</v>
       </c>
       <c r="D66">
@@ -5228,57 +5304,57 @@
         <v>14</v>
       </c>
       <c r="J66" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K66" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K66" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L66" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L66" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M66" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M66" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N66" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N66" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 66</v>
+      </c>
+      <c r="O66" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 66</v>
-      </c>
-      <c r="O66" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 66</v>
+      </c>
+      <c r="P66" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 66</v>
-      </c>
-      <c r="P66" s="4">
+        <v>66</v>
+      </c>
+      <c r="Q66" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>66</v>
-      </c>
-      <c r="Q66" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R66" s="6" t="str">
+        <f t="shared" si="12"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 66.xlsx</v>
+      </c>
+      <c r="S66" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R66" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T66" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 66.xlsx</v>
-      </c>
-      <c r="S66" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T66" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B73" si="36">"Cliente "&amp;ROW()</f>
+        <f t="shared" ref="B67:B73" si="34">"Cliente "&amp;ROW()</f>
         <v>Cliente 67</v>
       </c>
       <c r="D67">
@@ -5300,57 +5376,57 @@
         <v>14</v>
       </c>
       <c r="J67" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K67" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K67" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L67" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L67" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M67" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M67" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N67" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N67" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 67</v>
+      </c>
+      <c r="O67" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 67</v>
-      </c>
-      <c r="O67" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 67</v>
+      </c>
+      <c r="P67" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 67</v>
-      </c>
-      <c r="P67" s="4">
+        <v>67</v>
+      </c>
+      <c r="Q67" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>67</v>
-      </c>
-      <c r="Q67" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R67" s="6" t="str">
+        <f t="shared" ref="R67:R73" si="35">J67&amp;"Procesado\"&amp;N67&amp;".xlsx"</f>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 67.xlsx</v>
+      </c>
+      <c r="S67" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R67" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T67" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 67.xlsx</v>
-      </c>
-      <c r="S67" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T67" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B68" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>Cliente 68</v>
       </c>
       <c r="D68">
@@ -5372,57 +5448,57 @@
         <v>14</v>
       </c>
       <c r="J68" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K68" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K68" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L68" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L68" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M68" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M68" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N68" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N68" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 68</v>
+      </c>
+      <c r="O68" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 68</v>
-      </c>
-      <c r="O68" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 68</v>
+      </c>
+      <c r="P68" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 68</v>
-      </c>
-      <c r="P68" s="4">
+        <v>68</v>
+      </c>
+      <c r="Q68" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>68</v>
-      </c>
-      <c r="Q68" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R68" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 68.xlsx</v>
+      </c>
+      <c r="S68" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R68" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T68" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 68.xlsx</v>
-      </c>
-      <c r="S68" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T68" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B69" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>Cliente 69</v>
       </c>
       <c r="D69">
@@ -5444,57 +5520,57 @@
         <v>14</v>
       </c>
       <c r="J69" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K69" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K69" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L69" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L69" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M69" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M69" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N69" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N69" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 69</v>
+      </c>
+      <c r="O69" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 69</v>
-      </c>
-      <c r="O69" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 69</v>
+      </c>
+      <c r="P69" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 69</v>
-      </c>
-      <c r="P69" s="4">
+        <v>69</v>
+      </c>
+      <c r="Q69" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>69</v>
-      </c>
-      <c r="Q69" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R69" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 69.xlsx</v>
+      </c>
+      <c r="S69" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R69" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T69" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 69.xlsx</v>
-      </c>
-      <c r="S69" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T69" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B70" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>Cliente 70</v>
       </c>
       <c r="D70">
@@ -5516,57 +5592,57 @@
         <v>14</v>
       </c>
       <c r="J70" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K70" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K70" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L70" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L70" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M70" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M70" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N70" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N70" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 70</v>
+      </c>
+      <c r="O70" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 70</v>
-      </c>
-      <c r="O70" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 70</v>
+      </c>
+      <c r="P70" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 70</v>
-      </c>
-      <c r="P70" s="4">
+        <v>70</v>
+      </c>
+      <c r="Q70" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>70</v>
-      </c>
-      <c r="Q70" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R70" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 70.xlsx</v>
+      </c>
+      <c r="S70" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R70" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T70" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 70.xlsx</v>
-      </c>
-      <c r="S70" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T70" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B71" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>Cliente 71</v>
       </c>
       <c r="D71">
@@ -5588,57 +5664,57 @@
         <v>14</v>
       </c>
       <c r="J71" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K71" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K71" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L71" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L71" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M71" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M71" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N71" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N71" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 71</v>
+      </c>
+      <c r="O71" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 71</v>
-      </c>
-      <c r="O71" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 71</v>
+      </c>
+      <c r="P71" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 71</v>
-      </c>
-      <c r="P71" s="4">
+        <v>71</v>
+      </c>
+      <c r="Q71" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>71</v>
-      </c>
-      <c r="Q71" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R71" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 71.xlsx</v>
+      </c>
+      <c r="S71" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R71" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T71" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 71.xlsx</v>
-      </c>
-      <c r="S71" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T71" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B72" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>Cliente 72</v>
       </c>
       <c r="D72">
@@ -5660,57 +5736,57 @@
         <v>14</v>
       </c>
       <c r="J72" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K72" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K72" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L72" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L72" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M72" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M72" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N72" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N72" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 72</v>
+      </c>
+      <c r="O72" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 72</v>
-      </c>
-      <c r="O72" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 72</v>
+      </c>
+      <c r="P72" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 72</v>
-      </c>
-      <c r="P72" s="4">
+        <v>72</v>
+      </c>
+      <c r="Q72" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>72</v>
-      </c>
-      <c r="Q72" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R72" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 72.xlsx</v>
+      </c>
+      <c r="S72" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R72" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T72" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 72.xlsx</v>
-      </c>
-      <c r="S72" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T72" s="4">
-        <f t="shared" si="33"/>
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="B73" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>Cliente 73</v>
       </c>
       <c r="D73">
@@ -5732,47 +5808,47 @@
         <v>14</v>
       </c>
       <c r="J73" s="4" t="str">
+        <f t="shared" si="22"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
+      </c>
+      <c r="K73" s="4" t="str">
         <f t="shared" si="23"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\</v>
-      </c>
-      <c r="K73" s="4" t="str">
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
+      </c>
+      <c r="L73" s="3" t="str">
         <f t="shared" si="24"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IIBB\</v>
-      </c>
-      <c r="L73" s="3" t="str">
+        <v>Julio 2023</v>
+      </c>
+      <c r="M73" s="3" t="str">
         <f t="shared" si="25"/>
-        <v>Julio 2023</v>
-      </c>
-      <c r="M73" s="3" t="str">
+        <v>202307</v>
+      </c>
+      <c r="N73" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>202307</v>
-      </c>
-      <c r="N73" s="3" t="str">
+        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 73</v>
+      </c>
+      <c r="O73" s="3" t="str">
         <f t="shared" si="27"/>
-        <v>0 - 30000000000 - WP IVA - 202307 - Cliente 73</v>
-      </c>
-      <c r="O73" s="3" t="str">
+        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 73</v>
+      </c>
+      <c r="P73" s="4">
         <f t="shared" si="28"/>
-        <v>0 - 30000000000 - WP IIBB - 202307 - Cliente 73</v>
-      </c>
-      <c r="P73" s="4">
+        <v>73</v>
+      </c>
+      <c r="Q73" s="4" t="str">
         <f t="shared" si="29"/>
-        <v>73</v>
-      </c>
-      <c r="Q73" s="4" t="str">
+        <v>0</v>
+      </c>
+      <c r="R73" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Procesado\0 - 30000000000 - WP IVA - 202307 - Cliente 73.xlsx</v>
+      </c>
+      <c r="S73" s="4">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R73" s="6" t="str">
+        <v>1</v>
+      </c>
+      <c r="T73" s="4">
         <f t="shared" si="31"/>
-        <v>F:\Libros Compras y Ventas\2023\202307\Papeles de Trabajo\IVA\Resultados\0 - 30000000000 - WP IVA - 202307 - Cliente 73.xlsx</v>
-      </c>
-      <c r="S73" s="4">
-        <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="T73" s="4">
-        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -5782,12 +5858,13 @@
     <sortCondition ref="Q2:Q73"/>
     <sortCondition ref="B2:B73"/>
   </sortState>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H73" xr:uid="{DEF14D53-B6C1-4E78-84CB-7DBEF58A0FD6}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>